<commit_message>
create project structure selenium-cucumber-java
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/Login.xlsx
+++ b/src/test/java/TestData/Login.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mydoc\selenium\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mydoc\selenium-cucumber-java\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189DAEC6-E972-4074-842A-3BA90F2FE045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46C92C3-9716-4082-8EAB-2B1D672616BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Email</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>fiky@usenobi.com</t>
-  </si>
-  <si>
     <t>Usenobi123#</t>
   </si>
   <si>
@@ -45,40 +42,38 @@
     <t>Usenobi123</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>ss</t>
+    <t>fiky@gmail.com</t>
+  </si>
+  <si>
+    <t>testCase</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>Login With Wrong Email</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Login With Wrong Password</t>
+  </si>
+  <si>
+    <t>Login Success</t>
+  </si>
+  <si>
+    <t>Coming Soon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,16 +96,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,88 +381,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>3</v>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{A4970124-69AF-487D-A452-BC9CB93E7FFE}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{45C71E0C-A7CA-4582-B932-AA27FA42797B}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{120D3641-B79A-4802-B866-E2BAF4A1B06E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>